<commit_message>
concat zip to dest
</commit_message>
<xml_diff>
--- a/db/pocino.xlsx
+++ b/db/pocino.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Destination</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Daytona Beach, FL 32117</t>
   </si>
   <si>
-    <t>Santa Fe Springs, CA 90670</t>
-  </si>
-  <si>
     <t>Tracy, CA 95304</t>
   </si>
   <si>
@@ -84,6 +81,12 @@
   </si>
   <si>
     <t>Milpitas, CA 95035</t>
+  </si>
+  <si>
+    <t>Boise, ID 83717</t>
+  </si>
+  <si>
+    <t>Loveland, CO 80538</t>
   </si>
 </sst>
 </file>
@@ -403,20 +406,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="16" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="16" width="3" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -475,13 +478,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>385</v>
+        <v>440</v>
       </c>
       <c r="C2" s="1">
-        <v>740</v>
+        <v>830</v>
       </c>
       <c r="D2" s="1">
-        <v>1080</v>
+        <v>1190</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -501,13 +504,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>375</v>
+        <v>425</v>
       </c>
       <c r="C3" s="1">
-        <v>720</v>
+        <v>805</v>
       </c>
       <c r="D3" s="1">
-        <v>1035</v>
+        <v>1340</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -527,13 +530,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>395</v>
+        <v>450</v>
       </c>
       <c r="C4" s="1">
-        <v>750</v>
+        <v>840</v>
       </c>
       <c r="D4" s="1">
-        <v>1080</v>
+        <v>1190</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -553,13 +556,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>450</v>
+        <v>515</v>
       </c>
       <c r="C5" s="1">
-        <v>850</v>
+        <v>955</v>
       </c>
       <c r="D5" s="1">
-        <v>1195</v>
+        <v>1315</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -579,13 +582,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>500</v>
+        <v>570</v>
       </c>
       <c r="C6" s="1">
-        <v>970</v>
+        <v>1085</v>
       </c>
       <c r="D6" s="1">
-        <v>1395</v>
+        <v>1535</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -605,13 +608,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>575</v>
+        <v>655</v>
       </c>
       <c r="C7" s="1">
-        <v>1110</v>
+        <v>1245</v>
       </c>
       <c r="D7" s="1">
-        <v>1635</v>
+        <v>1790</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -631,65 +634,41 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>300</v>
+        <v>395</v>
       </c>
       <c r="C8" s="1">
-        <v>300</v>
+        <v>530</v>
       </c>
       <c r="D8" s="1">
-        <v>300</v>
+        <v>665</v>
       </c>
       <c r="E8" s="1">
-        <v>315</v>
+        <v>785</v>
       </c>
       <c r="F8" s="1">
-        <v>315</v>
-      </c>
-      <c r="G8" s="1">
-        <v>315</v>
-      </c>
-      <c r="H8" s="1">
-        <v>325</v>
-      </c>
-      <c r="I8" s="1">
-        <v>325</v>
-      </c>
-      <c r="J8" s="1">
-        <v>325</v>
-      </c>
-      <c r="K8" s="1">
-        <v>325</v>
-      </c>
-      <c r="L8" s="1">
-        <v>355</v>
-      </c>
-      <c r="M8" s="1">
-        <v>365</v>
-      </c>
-      <c r="N8" s="1">
-        <v>380</v>
-      </c>
-      <c r="O8" s="1">
-        <v>395</v>
-      </c>
-      <c r="P8" s="1">
-        <v>410</v>
-      </c>
+        <v>880</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1">
-        <v>495</v>
-      </c>
-      <c r="D9" s="1">
-        <v>620</v>
-      </c>
-      <c r="E9" s="1">
-        <v>735</v>
-      </c>
+      <c r="B9" s="1">
+        <v>485</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -707,13 +686,23 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>425</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+        <v>395</v>
+      </c>
+      <c r="C10" s="1">
+        <v>530</v>
+      </c>
+      <c r="D10" s="1">
+        <v>665</v>
+      </c>
+      <c r="E10" s="1">
+        <v>785</v>
+      </c>
+      <c r="F10" s="1">
+        <v>880</v>
+      </c>
+      <c r="G10" s="1">
+        <v>980</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -728,23 +717,13 @@
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
-        <v>345</v>
-      </c>
-      <c r="C11" s="1">
-        <v>465</v>
-      </c>
-      <c r="D11" s="1">
-        <v>590</v>
-      </c>
-      <c r="E11" s="1">
-        <v>695</v>
-      </c>
-      <c r="F11" s="1">
-        <v>785</v>
-      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
       <c r="G11" s="1">
-        <v>875</v>
+        <v>1800</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -763,11 +742,11 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1">
+        <v>1435</v>
+      </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="1">
-        <v>1580</v>
-      </c>
+      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -782,14 +761,24 @@
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="B13" s="1">
+        <v>335</v>
+      </c>
+      <c r="C13" s="1">
+        <v>480</v>
+      </c>
+      <c r="D13" s="1">
+        <v>610</v>
+      </c>
       <c r="E13" s="1">
-        <v>1260</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+        <v>700</v>
+      </c>
+      <c r="F13" s="1">
+        <v>840</v>
+      </c>
+      <c r="G13" s="1">
+        <v>975</v>
+      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -805,27 +794,35 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>295</v>
+        <v>400</v>
       </c>
       <c r="C14" s="1">
-        <v>420</v>
+        <v>540</v>
       </c>
       <c r="D14" s="1">
-        <v>540</v>
+        <v>690</v>
       </c>
       <c r="E14" s="1">
-        <v>620</v>
+        <v>820</v>
       </c>
       <c r="F14" s="1">
-        <v>750</v>
+        <v>910</v>
       </c>
       <c r="G14" s="1">
-        <v>870</v>
-      </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+        <v>1000</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1050</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1105</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1150</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1200</v>
+      </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -837,35 +834,27 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>350</v>
+        <v>395</v>
       </c>
       <c r="C15" s="1">
-        <v>475</v>
+        <v>530</v>
       </c>
       <c r="D15" s="1">
-        <v>610</v>
+        <v>665</v>
       </c>
       <c r="E15" s="1">
-        <v>725</v>
+        <v>785</v>
       </c>
       <c r="F15" s="1">
-        <v>815</v>
+        <v>880</v>
       </c>
       <c r="G15" s="1">
-        <v>895</v>
-      </c>
-      <c r="H15" s="1">
-        <v>945</v>
-      </c>
-      <c r="I15" s="1">
-        <v>995</v>
-      </c>
-      <c r="J15" s="1">
-        <v>1045</v>
-      </c>
-      <c r="K15" s="1">
-        <v>1090</v>
-      </c>
+        <v>980</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -877,22 +866,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>345</v>
+        <v>395</v>
       </c>
       <c r="C16" s="1">
-        <v>465</v>
+        <v>530</v>
       </c>
       <c r="D16" s="1">
-        <v>590</v>
+        <v>665</v>
       </c>
       <c r="E16" s="1">
-        <v>695</v>
+        <v>785</v>
       </c>
       <c r="F16" s="1">
-        <v>785</v>
+        <v>880</v>
       </c>
       <c r="G16" s="1">
-        <v>875</v>
+        <v>980</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -909,22 +898,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>345</v>
+        <v>400</v>
       </c>
       <c r="C17" s="1">
-        <v>465</v>
+        <v>565</v>
       </c>
       <c r="D17" s="1">
-        <v>590</v>
+        <v>705</v>
       </c>
       <c r="E17" s="1">
-        <v>695</v>
+        <v>835</v>
       </c>
       <c r="F17" s="1">
-        <v>785</v>
+        <v>930</v>
       </c>
       <c r="G17" s="1">
-        <v>875</v>
+        <v>1030</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -941,22 +930,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>350</v>
+        <v>400</v>
       </c>
       <c r="C18" s="1">
-        <v>495</v>
+        <v>565</v>
       </c>
       <c r="D18" s="1">
-        <v>620</v>
+        <v>705</v>
       </c>
       <c r="E18" s="1">
-        <v>735</v>
+        <v>835</v>
       </c>
       <c r="F18" s="1">
-        <v>815</v>
+        <v>930</v>
       </c>
       <c r="G18" s="1">
-        <v>905</v>
+        <v>1030</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -973,22 +962,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>350</v>
+        <v>400</v>
       </c>
       <c r="C19" s="1">
-        <v>495</v>
+        <v>565</v>
       </c>
       <c r="D19" s="1">
-        <v>620</v>
+        <v>705</v>
       </c>
       <c r="E19" s="1">
-        <v>735</v>
+        <v>835</v>
       </c>
       <c r="F19" s="1">
-        <v>815</v>
+        <v>930</v>
       </c>
       <c r="G19" s="1">
-        <v>905</v>
+        <v>1030</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -1004,33 +993,17 @@
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="1">
-        <v>350</v>
-      </c>
       <c r="C20" s="1">
-        <v>495</v>
-      </c>
-      <c r="D20" s="1">
-        <v>620</v>
-      </c>
-      <c r="E20" s="1">
-        <v>735</v>
-      </c>
-      <c r="F20" s="1">
-        <v>815</v>
-      </c>
-      <c r="G20" s="1">
-        <v>905</v>
-      </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>540</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>